<commit_message>
Updated performance test data
Former-commit-id: 5fd1377adb9dc4b83deac609f8ba35e873b1ec88 [formerly e0d274f78ef6a95b396a8a9cb27550f61a95fb0b]
Former-commit-id: ca979071432c7c2aa4d947a2944387358d114a3c
</commit_message>
<xml_diff>
--- a/Timing tests build 0.7.2.0.xlsx
+++ b/Timing tests build 0.7.2.0.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="26">
   <si>
     <t>Test:</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>Times in milliseconds</t>
+  </si>
+  <si>
+    <t>UWP Windows 10 Mobile App (Edge Engine 15.15063)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windows 10 Mobile 10.0.15063.414 on Lumia 950XL </t>
   </si>
 </sst>
 </file>
@@ -134,7 +140,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,6 +159,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -167,7 +179,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -202,26 +214,20 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <numFmt numFmtId="4" formatCode="#,##0.00"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -242,6 +248,41 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -276,17 +317,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B9:G12" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B9:G12" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="B9:G12"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Event"/>
     <tableColumn id="2" name="CSS from ZIM (ms) baseline"/>
     <tableColumn id="3" name="CSS from cache (desktop CSS)"/>
-    <tableColumn id="5" name="CSS DT gain to baseline" dataDxfId="3">
+    <tableColumn id="5" name="CSS DT gain to baseline" dataDxfId="7">
       <calculatedColumnFormula>"+" &amp; ROUND((Table1[[#This Row],[CSS from ZIM (ms) baseline]]-Table1[[#This Row],[CSS from cache (desktop CSS)]])/Table1[[#This Row],[CSS from cache (desktop CSS)]]*100,1) &amp; "%"</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="CSS from cache (mobile  xform)"/>
-    <tableColumn id="6" name="CSS MB gain to baseline" dataDxfId="1">
+    <tableColumn id="6" name="CSS MB gain to baseline" dataDxfId="6">
       <calculatedColumnFormula>"+" &amp; ROUND((Table1[[#This Row],[CSS from ZIM (ms) baseline]]-Table1[[#This Row],[CSS from cache (mobile  xform)]])/Table1[[#This Row],[CSS from cache (mobile  xform)]]*100,1) &amp; "%"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -295,21 +336,40 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="B25:G28" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="B25:G28" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="B25:G28"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Event"/>
     <tableColumn id="2" name="CSS from ZIM (ms) baseline"/>
     <tableColumn id="3" name="CSS from cache (desktop CSS)"/>
-    <tableColumn id="5" name="CSS DT gain to baseline" dataDxfId="2">
+    <tableColumn id="5" name="CSS DT gain to baseline" dataDxfId="4">
       <calculatedColumnFormula>"+" &amp; ROUND((Table14[[#This Row],[CSS from ZIM (ms) baseline]]-Table14[[#This Row],[CSS from cache (desktop CSS)]])/Table14[[#This Row],[CSS from cache (desktop CSS)]]*100,1) &amp; "%"</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="CSS from cache (mobile  xform)"/>
-    <tableColumn id="6" name="CSS MB gain to baseline" dataDxfId="0">
+    <tableColumn id="6" name="CSS MB gain to baseline" dataDxfId="3">
       <calculatedColumnFormula>"+" &amp; ROUND((Table14[[#This Row],[CSS from ZIM (ms) baseline]]-Table14[[#This Row],[CSS from cache (mobile  xform)]])/Table14[[#This Row],[CSS from cache (mobile  xform)]]*100,1) &amp; "%"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table143" displayName="Table143" ref="B37:G40" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="B37:G40"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Event"/>
+    <tableColumn id="2" name="CSS from ZIM (ms) baseline"/>
+    <tableColumn id="3" name="CSS from cache (desktop CSS)"/>
+    <tableColumn id="5" name="CSS DT gain to baseline" dataDxfId="1">
+      <calculatedColumnFormula>"+" &amp; ROUND((Table143[[#This Row],[CSS from ZIM (ms) baseline]]-Table143[[#This Row],[CSS from cache (desktop CSS)]])/Table143[[#This Row],[CSS from cache (desktop CSS)]]*100,1) &amp; "%"</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="CSS from cache (mobile  xform)"/>
+    <tableColumn id="6" name="CSS MB gain to baseline" dataDxfId="0">
+      <calculatedColumnFormula>"+" &amp; ROUND((Table143[[#This Row],[CSS from ZIM (ms) baseline]]-Table143[[#This Row],[CSS from cache (mobile  xform)]])/Table143[[#This Row],[CSS from cache (mobile  xform)]]*100,1) &amp; "%"</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -610,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G28"/>
+  <dimension ref="B3:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -943,12 +1003,164 @@
         <v>+41.4%</v>
       </c>
     </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B31" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B32" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G32" s="19"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B33" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B34" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B35" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+    </row>
+    <row r="37" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B37" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="2">
+        <v>5152.8500000000004</v>
+      </c>
+      <c r="D38" s="2">
+        <v>4935.7700000000004</v>
+      </c>
+      <c r="E38" s="11" t="str">
+        <f>"+" &amp; ROUND((Table143[[#This Row],[CSS from ZIM (ms) baseline]]-Table143[[#This Row],[CSS from cache (desktop CSS)]])/Table143[[#This Row],[CSS from cache (desktop CSS)]]*100,1) &amp; "%"</f>
+        <v>+4.4%</v>
+      </c>
+      <c r="F38" s="2">
+        <v>4940.18</v>
+      </c>
+      <c r="G38" s="11" t="str">
+        <f>"+" &amp; ROUND((Table143[[#This Row],[CSS from ZIM (ms) baseline]]-Table143[[#This Row],[CSS from cache (mobile  xform)]])/Table143[[#This Row],[CSS from cache (mobile  xform)]]*100,1) &amp; "%"</f>
+        <v>+4.3%</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="2">
+        <v>30980.57</v>
+      </c>
+      <c r="D39" s="4">
+        <v>1297.31</v>
+      </c>
+      <c r="E39" s="15" t="str">
+        <f>"+" &amp; ROUND((Table143[[#This Row],[CSS from ZIM (ms) baseline]]-Table143[[#This Row],[CSS from cache (desktop CSS)]])/Table143[[#This Row],[CSS from cache (desktop CSS)]]*100,1) &amp; "%"</f>
+        <v>+2288.1%</v>
+      </c>
+      <c r="F39" s="2">
+        <v>9250.73</v>
+      </c>
+      <c r="G39" s="14" t="str">
+        <f>"+" &amp; ROUND((Table143[[#This Row],[CSS from ZIM (ms) baseline]]-Table143[[#This Row],[CSS from cache (mobile  xform)]])/Table143[[#This Row],[CSS from cache (mobile  xform)]]*100,1) &amp; "%"</f>
+        <v>+234.9%</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="3">
+        <f>C38+C39</f>
+        <v>36133.42</v>
+      </c>
+      <c r="D40" s="3">
+        <f>D38+D39</f>
+        <v>6233.08</v>
+      </c>
+      <c r="E40" s="13" t="str">
+        <f>"+" &amp; ROUND((Table143[[#This Row],[CSS from ZIM (ms) baseline]]-Table143[[#This Row],[CSS from cache (desktop CSS)]])/Table143[[#This Row],[CSS from cache (desktop CSS)]]*100,1) &amp; "%"</f>
+        <v>+479.7%</v>
+      </c>
+      <c r="F40" s="16">
+        <f>F38+F39</f>
+        <v>14190.91</v>
+      </c>
+      <c r="G40" s="17" t="str">
+        <f>"+" &amp; ROUND((Table143[[#This Row],[CSS from ZIM (ms) baseline]]-Table143[[#This Row],[CSS from cache (mobile  xform)]])/Table143[[#This Row],[CSS from cache (mobile  xform)]]*100,1) &amp; "%"</f>
+        <v>+154.6%</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adds timers and updates timing tests
Former-commit-id: 97b1841cca2cd46a843e157988d92b179734218d [formerly 3680603734b09be686957e2d25ebc2653de68c9d]
Former-commit-id: c2086c68ba32b606516c650191788c70752e64bb
</commit_message>
<xml_diff>
--- a/Timing tests build 0.7.2.0.xlsx
+++ b/Timing tests build 0.7.2.0.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="30">
   <si>
     <t>Test:</t>
   </si>
@@ -78,9 +78,6 @@
     <t>CSS from cache (desktop CSS)</t>
   </si>
   <si>
-    <t>Total from click to CSS rendered</t>
-  </si>
-  <si>
     <t>Firefox 54.0.1 (32bit)</t>
   </si>
   <si>
@@ -103,6 +100,21 @@
   </si>
   <si>
     <t xml:space="preserve">Windows 10 Mobile 10.0.15063.414 on Lumia 950XL </t>
+  </si>
+  <si>
+    <t>Time to Document Ready</t>
+  </si>
+  <si>
+    <t>Total to render 6 CSS sheets</t>
+  </si>
+  <si>
+    <t>Time to Document Ready = total time from click on article title to render of last image</t>
+  </si>
+  <si>
+    <t>Time to extract 253 images</t>
+  </si>
+  <si>
+    <t>Total to extract 6 CSS sheets</t>
   </si>
 </sst>
 </file>
@@ -179,7 +191,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -216,6 +228,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -317,8 +341,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B9:G12" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="B9:G12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B9:G14" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="B9:G14"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Event"/>
     <tableColumn id="2" name="CSS from ZIM (ms) baseline"/>
@@ -336,8 +360,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="B25:G28" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="B25:G28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="B27:G32" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="B27:G32"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Event"/>
     <tableColumn id="2" name="CSS from ZIM (ms) baseline"/>
@@ -355,8 +379,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table143" displayName="Table143" ref="B37:G40" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="B37:G40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table143" displayName="Table143" ref="B45:G50" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="B45:G50"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Event"/>
     <tableColumn id="2" name="CSS from ZIM (ms) baseline"/>
@@ -670,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G44"/>
+  <dimension ref="B3:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -708,7 +732,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G4" s="7"/>
     </row>
@@ -753,19 +777,19 @@
         <v>3</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.45">
@@ -814,17 +838,17 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="3">
+        <v>26</v>
+      </c>
+      <c r="C12" s="16">
         <f>C10+C11</f>
         <v>15128.259999999998</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="16">
         <f>D10+D11</f>
         <v>2613.0149999999999</v>
       </c>
-      <c r="E12" s="13" t="str">
+      <c r="E12" s="17" t="str">
         <f>"+" &amp; ROUND((Table1[[#This Row],[CSS from ZIM (ms) baseline]]-Table1[[#This Row],[CSS from cache (desktop CSS)]])/Table1[[#This Row],[CSS from cache (desktop CSS)]]*100,1) &amp; "%"</f>
         <v>+479%</v>
       </c>
@@ -837,53 +861,79 @@
         <v>+190.3%</v>
       </c>
     </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="16">
+        <f>C14-C12</f>
+        <v>8157.41</v>
+      </c>
+      <c r="D13" s="16">
+        <f>D14-D12</f>
+        <v>6472.84</v>
+      </c>
+      <c r="E13" s="22" t="str">
+        <f>"+" &amp; ROUND((Table1[[#This Row],[CSS from ZIM (ms) baseline]]-Table1[[#This Row],[CSS from cache (desktop CSS)]])/Table1[[#This Row],[CSS from cache (desktop CSS)]]*100,1) &amp; "%"</f>
+        <v>+26%</v>
+      </c>
+      <c r="F13" s="16">
+        <f>F14-F12</f>
+        <v>3871.54</v>
+      </c>
+      <c r="G13" s="17" t="str">
+        <f>"+" &amp; ROUND((Table1[[#This Row],[CSS from ZIM (ms) baseline]]-Table1[[#This Row],[CSS from cache (mobile  xform)]])/Table1[[#This Row],[CSS from cache (mobile  xform)]]*100,1) &amp; "%"</f>
+        <v>+110.7%</v>
+      </c>
+    </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="3">
+        <v>23285.67</v>
+      </c>
+      <c r="D14" s="3">
+        <v>9085.8549999999996</v>
+      </c>
+      <c r="E14" s="21" t="str">
+        <f>"+" &amp; ROUND((Table1[[#This Row],[CSS from ZIM (ms) baseline]]-Table1[[#This Row],[CSS from cache (desktop CSS)]])/Table1[[#This Row],[CSS from cache (desktop CSS)]]*100,1) &amp; "%"</f>
+        <v>+156.3%</v>
+      </c>
+      <c r="F14" s="16">
+        <v>9082.875</v>
+      </c>
+      <c r="G14" s="17" t="str">
+        <f>"+" &amp; ROUND((Table1[[#This Row],[CSS from ZIM (ms) baseline]]-Table1[[#This Row],[CSS from cache (mobile  xform)]])/Table1[[#This Row],[CSS from cache (mobile  xform)]]*100,1) &amp; "%"</f>
+        <v>+156.4%</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B15" t="s">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B16" t="s">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B19" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B20" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" s="10"/>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B21" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -892,281 +942,426 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B22" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>18</v>
+        <v>1</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>2</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="F22" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="G22" s="10"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B23" s="9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
     </row>
-    <row r="25" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B25" s="6" t="s">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B24" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B25" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+    </row>
+    <row r="27" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B27" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G25" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B26" t="s">
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B28" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C28" s="2">
         <v>319.04000000000002</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D28" s="2">
         <v>293.94</v>
       </c>
-      <c r="E26" s="11" t="str">
+      <c r="E28" s="11" t="str">
         <f>"+" &amp; ROUND((Table14[[#This Row],[CSS from ZIM (ms) baseline]]-Table14[[#This Row],[CSS from cache (desktop CSS)]])/Table14[[#This Row],[CSS from cache (desktop CSS)]]*100,1) &amp; "%"</f>
         <v>+8.5%</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F28" s="2">
         <v>317.58999999999997</v>
       </c>
-      <c r="G26" s="11" t="str">
+      <c r="G28" s="11" t="str">
         <f>"+" &amp; ROUND((Table14[[#This Row],[CSS from ZIM (ms) baseline]]-Table14[[#This Row],[CSS from cache (mobile  xform)]])/Table14[[#This Row],[CSS from cache (mobile  xform)]]*100,1) &amp; "%"</f>
         <v>+0.5%</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B27" t="s">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B29" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C29" s="2">
         <v>1053.74</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D29" s="4">
         <v>469.34</v>
       </c>
-      <c r="E27" s="15" t="str">
+      <c r="E29" s="15" t="str">
         <f>"+" &amp; ROUND((Table14[[#This Row],[CSS from ZIM (ms) baseline]]-Table14[[#This Row],[CSS from cache (desktop CSS)]])/Table14[[#This Row],[CSS from cache (desktop CSS)]]*100,1) &amp; "%"</f>
         <v>+124.5%</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F29" s="2">
         <v>653.02</v>
       </c>
-      <c r="G27" s="14" t="str">
+      <c r="G29" s="14" t="str">
         <f>"+" &amp; ROUND((Table14[[#This Row],[CSS from ZIM (ms) baseline]]-Table14[[#This Row],[CSS from cache (mobile  xform)]])/Table14[[#This Row],[CSS from cache (mobile  xform)]]*100,1) &amp; "%"</f>
         <v>+61.4%</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="3">
-        <f>C26+C27</f>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="16">
+        <f>C28+C29</f>
         <v>1372.78</v>
       </c>
-      <c r="D28" s="3">
-        <f>D26+D27</f>
+      <c r="D30" s="16">
+        <f>D28+D29</f>
         <v>763.28</v>
       </c>
-      <c r="E28" s="13" t="str">
+      <c r="E30" s="17" t="str">
         <f>"+" &amp; ROUND((Table14[[#This Row],[CSS from ZIM (ms) baseline]]-Table14[[#This Row],[CSS from cache (desktop CSS)]])/Table14[[#This Row],[CSS from cache (desktop CSS)]]*100,1) &amp; "%"</f>
         <v>+79.9%</v>
       </c>
-      <c r="F28" s="16">
-        <f>F26+F27</f>
+      <c r="F30" s="16">
+        <f>F28+F29</f>
         <v>970.6099999999999</v>
       </c>
-      <c r="G28" s="17" t="str">
+      <c r="G30" s="17" t="str">
         <f>"+" &amp; ROUND((Table14[[#This Row],[CSS from ZIM (ms) baseline]]-Table14[[#This Row],[CSS from cache (mobile  xform)]])/Table14[[#This Row],[CSS from cache (mobile  xform)]]*100,1) &amp; "%"</f>
         <v>+41.4%</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B31" s="18" t="s">
+      <c r="B31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="16">
+        <f>C32-C30</f>
+        <v>5073.67</v>
+      </c>
+      <c r="D31" s="16">
+        <f>D32-D30</f>
+        <v>4071.5200000000004</v>
+      </c>
+      <c r="E31" s="23" t="str">
+        <f>"+" &amp; ROUND((Table14[[#This Row],[CSS from ZIM (ms) baseline]]-Table14[[#This Row],[CSS from cache (desktop CSS)]])/Table14[[#This Row],[CSS from cache (desktop CSS)]]*100,1) &amp; "%"</f>
+        <v>+24.6%</v>
+      </c>
+      <c r="F31" s="16">
+        <f>F32-F30</f>
+        <v>4289.33</v>
+      </c>
+      <c r="G31" s="17" t="str">
+        <f>"+" &amp; ROUND((Table14[[#This Row],[CSS from ZIM (ms) baseline]]-Table14[[#This Row],[CSS from cache (mobile  xform)]])/Table14[[#This Row],[CSS from cache (mobile  xform)]]*100,1) &amp; "%"</f>
+        <v>+18.3%</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="3">
+        <v>6446.45</v>
+      </c>
+      <c r="D32" s="3">
+        <v>4834.8</v>
+      </c>
+      <c r="E32" s="20" t="str">
+        <f>"+" &amp; ROUND((Table14[[#This Row],[CSS from ZIM (ms) baseline]]-Table14[[#This Row],[CSS from cache (desktop CSS)]])/Table14[[#This Row],[CSS from cache (desktop CSS)]]*100,1) &amp; "%"</f>
+        <v>+33.3%</v>
+      </c>
+      <c r="F32" s="16">
+        <v>5259.94</v>
+      </c>
+      <c r="G32" s="17" t="str">
+        <f>"+" &amp; ROUND((Table14[[#This Row],[CSS from ZIM (ms) baseline]]-Table14[[#This Row],[CSS from cache (mobile  xform)]])/Table14[[#This Row],[CSS from cache (mobile  xform)]]*100,1) &amp; "%"</f>
+        <v>+22.6%</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B34" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B39" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C39" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B32" s="18" t="s">
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B40" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="C40" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19" t="s">
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G40" s="19"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B41" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B42" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G32" s="19"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B33" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B34" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="18" t="s">
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B43" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B35" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-    </row>
-    <row r="37" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B37" s="6" t="s">
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+    </row>
+    <row r="45" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B45" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C45" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E37" s="5" t="s">
+      <c r="F45" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="G45" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G37" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B38" t="s">
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B46" t="s">
         <v>7</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C46" s="2">
         <v>5152.8500000000004</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D46" s="2">
         <v>4935.7700000000004</v>
       </c>
-      <c r="E38" s="11" t="str">
+      <c r="E46" s="11" t="str">
         <f>"+" &amp; ROUND((Table143[[#This Row],[CSS from ZIM (ms) baseline]]-Table143[[#This Row],[CSS from cache (desktop CSS)]])/Table143[[#This Row],[CSS from cache (desktop CSS)]]*100,1) &amp; "%"</f>
         <v>+4.4%</v>
       </c>
-      <c r="F38" s="2">
+      <c r="F46" s="2">
         <v>4940.18</v>
       </c>
-      <c r="G38" s="11" t="str">
+      <c r="G46" s="11" t="str">
         <f>"+" &amp; ROUND((Table143[[#This Row],[CSS from ZIM (ms) baseline]]-Table143[[#This Row],[CSS from cache (mobile  xform)]])/Table143[[#This Row],[CSS from cache (mobile  xform)]]*100,1) &amp; "%"</f>
         <v>+4.3%</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B39" t="s">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B47" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C47" s="2">
         <v>30980.57</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D47" s="4">
         <v>1297.31</v>
       </c>
-      <c r="E39" s="15" t="str">
+      <c r="E47" s="15" t="str">
         <f>"+" &amp; ROUND((Table143[[#This Row],[CSS from ZIM (ms) baseline]]-Table143[[#This Row],[CSS from cache (desktop CSS)]])/Table143[[#This Row],[CSS from cache (desktop CSS)]]*100,1) &amp; "%"</f>
         <v>+2288.1%</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F47" s="2">
         <v>9250.73</v>
       </c>
-      <c r="G39" s="14" t="str">
+      <c r="G47" s="14" t="str">
         <f>"+" &amp; ROUND((Table143[[#This Row],[CSS from ZIM (ms) baseline]]-Table143[[#This Row],[CSS from cache (mobile  xform)]])/Table143[[#This Row],[CSS from cache (mobile  xform)]]*100,1) &amp; "%"</f>
         <v>+234.9%</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C40" s="3">
-        <f>C38+C39</f>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B48" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" s="3">
+        <f>C46+C47</f>
         <v>36133.42</v>
       </c>
-      <c r="D40" s="3">
-        <f>D38+D39</f>
+      <c r="D48" s="3">
+        <f>D46+D47</f>
         <v>6233.08</v>
       </c>
-      <c r="E40" s="13" t="str">
+      <c r="E48" s="13" t="str">
         <f>"+" &amp; ROUND((Table143[[#This Row],[CSS from ZIM (ms) baseline]]-Table143[[#This Row],[CSS from cache (desktop CSS)]])/Table143[[#This Row],[CSS from cache (desktop CSS)]]*100,1) &amp; "%"</f>
         <v>+479.7%</v>
       </c>
-      <c r="F40" s="16">
-        <f>F38+F39</f>
+      <c r="F48" s="16">
+        <f>F46+F47</f>
         <v>14190.91</v>
       </c>
-      <c r="G40" s="17" t="str">
+      <c r="G48" s="17" t="str">
         <f>"+" &amp; ROUND((Table143[[#This Row],[CSS from ZIM (ms) baseline]]-Table143[[#This Row],[CSS from cache (mobile  xform)]])/Table143[[#This Row],[CSS from cache (mobile  xform)]]*100,1) &amp; "%"</f>
         <v>+154.6%</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B42" s="1" t="s">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B49" t="s">
+        <v>28</v>
+      </c>
+      <c r="C49" s="16">
+        <f>C50-C48</f>
+        <v>27117.43</v>
+      </c>
+      <c r="D49" s="16">
+        <f>D50-D48</f>
+        <v>22202.614999999998</v>
+      </c>
+      <c r="E49" s="20" t="str">
+        <f>"+" &amp; ROUND((Table143[[#This Row],[CSS from ZIM (ms) baseline]]-Table143[[#This Row],[CSS from cache (desktop CSS)]])/Table143[[#This Row],[CSS from cache (desktop CSS)]]*100,1) &amp; "%"</f>
+        <v>+22.1%</v>
+      </c>
+      <c r="F49" s="16">
+        <f>F50-F48</f>
+        <v>13136.355</v>
+      </c>
+      <c r="G49" s="17" t="str">
+        <f>"+" &amp; ROUND((Table143[[#This Row],[CSS from ZIM (ms) baseline]]-Table143[[#This Row],[CSS from cache (mobile  xform)]])/Table143[[#This Row],[CSS from cache (mobile  xform)]]*100,1) &amp; "%"</f>
+        <v>+106.4%</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B50" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" s="3">
+        <v>63250.85</v>
+      </c>
+      <c r="D50" s="3">
+        <v>28435.695</v>
+      </c>
+      <c r="E50" s="20" t="str">
+        <f>"+" &amp; ROUND((Table143[[#This Row],[CSS from ZIM (ms) baseline]]-Table143[[#This Row],[CSS from cache (desktop CSS)]])/Table143[[#This Row],[CSS from cache (desktop CSS)]]*100,1) &amp; "%"</f>
+        <v>+122.4%</v>
+      </c>
+      <c r="F50" s="16">
+        <v>27327.264999999999</v>
+      </c>
+      <c r="G50" s="17" t="str">
+        <f>"+" &amp; ROUND((Table143[[#This Row],[CSS from ZIM (ms) baseline]]-Table143[[#This Row],[CSS from cache (mobile  xform)]])/Table143[[#This Row],[CSS from cache (mobile  xform)]]*100,1) &amp; "%"</f>
+        <v>+131.5%</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B52" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B43" t="s">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B53" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B44" t="s">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B54" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B55" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>